<commit_message>
pagination fix applied - Missing Rotherham etc
</commit_message>
<xml_diff>
--- a/ofsted_csc_send_overview.xlsx
+++ b/ofsted_csc_send_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="584">
   <si>
     <t>80428</t>
   </si>
@@ -1181,6 +1181,543 @@
   </si>
   <si>
     <t>25/09/24</t>
+  </si>
+  <si>
+    <t>80534</t>
+  </si>
+  <si>
+    <t>891</t>
+  </si>
+  <si>
+    <t>E10000024</t>
+  </si>
+  <si>
+    <t>896, 909, 830, 881, 886, 888, 925, 940, 860, 885</t>
+  </si>
+  <si>
+    <t>nottinghamshire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50216722</t>
+  </si>
+  <si>
+    <t>24/06/2016</t>
+  </si>
+  <si>
+    <t>30/01/23</t>
+  </si>
+  <si>
+    <t>03/02/23</t>
+  </si>
+  <si>
+    <t>30/07/24</t>
+  </si>
+  <si>
+    <t>There are widespread and/or systemic failings leading to significant concerns about the experiences and outcomes of children and young people with special educational needs and/or disabilities (SEND) which the local area partnership must address urgently.  A monitoring inspection will be carried out within approximately 18 months. The next full area SEND inspection will take place within approximately 3 years.</t>
+  </si>
+  <si>
+    <t>80535</t>
+  </si>
+  <si>
+    <t>353</t>
+  </si>
+  <si>
+    <t>E08000004</t>
+  </si>
+  <si>
+    <t>889, 350, 380, 831, 332, 382, 354, 372, 357, 335</t>
+  </si>
+  <si>
+    <t>oldham</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50226808</t>
+  </si>
+  <si>
+    <t>26/06/23</t>
+  </si>
+  <si>
+    <t>30/06/23</t>
+  </si>
+  <si>
+    <t>29/08/23</t>
+  </si>
+  <si>
+    <t>26/12/24</t>
+  </si>
+  <si>
+    <t>80536</t>
+  </si>
+  <si>
+    <t>931</t>
+  </si>
+  <si>
+    <t>E10000025</t>
+  </si>
+  <si>
+    <t>800, 867, 825, 873, 916, 850, 919, 869, 938, 865</t>
+  </si>
+  <si>
+    <t>oxfordshire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50228374</t>
+  </si>
+  <si>
+    <t>13/07/23</t>
+  </si>
+  <si>
+    <t>21/07/23</t>
+  </si>
+  <si>
+    <t>15/09/23</t>
+  </si>
+  <si>
+    <t>13/01/25</t>
+  </si>
+  <si>
+    <t>80538</t>
+  </si>
+  <si>
+    <t>879</t>
+  </si>
+  <si>
+    <t>E06000026</t>
+  </si>
+  <si>
+    <t>839, 921, 887, 874, 851, 372, 882, 357, 894, 880</t>
+  </si>
+  <si>
+    <t>plymouth</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50226534</t>
+  </si>
+  <si>
+    <t>14/10/2016</t>
+  </si>
+  <si>
+    <t>22/08/23</t>
+  </si>
+  <si>
+    <t>80543</t>
+  </si>
+  <si>
+    <t>372</t>
+  </si>
+  <si>
+    <t>E08000018</t>
+  </si>
+  <si>
+    <t>370, 371, 332, 812, 813, 807, 357, 894, 384, 359</t>
+  </si>
+  <si>
+    <t>rotherham</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50261626</t>
+  </si>
+  <si>
+    <t>30/09/24</t>
+  </si>
+  <si>
+    <t>04/10/24</t>
+  </si>
+  <si>
+    <t>30/09/29</t>
+  </si>
+  <si>
+    <t>80547</t>
+  </si>
+  <si>
+    <t>857</t>
+  </si>
+  <si>
+    <t>E06000017</t>
+  </si>
+  <si>
+    <t>825, 873, 823, 895, 850, 815, 931, 937, 869, 865</t>
+  </si>
+  <si>
+    <t>rutland</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50225252</t>
+  </si>
+  <si>
+    <t>15/05/23</t>
+  </si>
+  <si>
+    <t>03/08/23</t>
+  </si>
+  <si>
+    <t>15/05/28</t>
+  </si>
+  <si>
+    <t>80549</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>E08000028</t>
+  </si>
+  <si>
+    <t>330, 889, 331, 831, 821, 892, 874, 861, 335, 336</t>
+  </si>
+  <si>
+    <t>sandwell</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50227802</t>
+  </si>
+  <si>
+    <t>21/03/2019</t>
+  </si>
+  <si>
+    <t>03/07/23</t>
+  </si>
+  <si>
+    <t>07/07/23</t>
+  </si>
+  <si>
+    <t>12/09/23</t>
+  </si>
+  <si>
+    <t>03/07/26</t>
+  </si>
+  <si>
+    <t>80558</t>
+  </si>
+  <si>
+    <t>852</t>
+  </si>
+  <si>
+    <t>E06000045</t>
+  </si>
+  <si>
+    <t>801, 331, 831, 810, 874, 879, 851, 355, 373, 861</t>
+  </si>
+  <si>
+    <t>southampton</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50252575</t>
+  </si>
+  <si>
+    <t>13/05/24</t>
+  </si>
+  <si>
+    <t>17/05/24</t>
+  </si>
+  <si>
+    <t>16/07/24</t>
+  </si>
+  <si>
+    <t>13/05/27</t>
+  </si>
+  <si>
+    <t>80559</t>
+  </si>
+  <si>
+    <t>882</t>
+  </si>
+  <si>
+    <t>E06000033</t>
+  </si>
+  <si>
+    <t>839, 845, 881, 921, 886, 887, 879, 935, 866, 894</t>
+  </si>
+  <si>
+    <t>southend-on-sea</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50219405</t>
+  </si>
+  <si>
+    <t>06/10/2018</t>
+  </si>
+  <si>
+    <t>06/03/23</t>
+  </si>
+  <si>
+    <t>10/03/23</t>
+  </si>
+  <si>
+    <t>09/06/23</t>
+  </si>
+  <si>
+    <t>06/03/26</t>
+  </si>
+  <si>
+    <t>80564</t>
+  </si>
+  <si>
+    <t>861</t>
+  </si>
+  <si>
+    <t>E06000021</t>
+  </si>
+  <si>
+    <t>370, 890, 371, 810, 806, 812, 354, 372, 357, 335</t>
+  </si>
+  <si>
+    <t>stoke-on-trent</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50243303</t>
+  </si>
+  <si>
+    <t>15/07/2016</t>
+  </si>
+  <si>
+    <t>29/01/27</t>
+  </si>
+  <si>
+    <t>80565</t>
+  </si>
+  <si>
+    <t>935</t>
+  </si>
+  <si>
+    <t>E10000029</t>
+  </si>
+  <si>
+    <t>908, 878, 838, 845, 916, 925, 926, 893, 933, 885</t>
+  </si>
+  <si>
+    <t>suffolk</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50238584</t>
+  </si>
+  <si>
+    <t>23/01/2019</t>
+  </si>
+  <si>
+    <t>13/11/23</t>
+  </si>
+  <si>
+    <t>17/11/23</t>
+  </si>
+  <si>
+    <t>30/01/24</t>
+  </si>
+  <si>
+    <t>13/05/25</t>
+  </si>
+  <si>
+    <t>80567</t>
+  </si>
+  <si>
+    <t>936</t>
+  </si>
+  <si>
+    <t>E10000030</t>
+  </si>
+  <si>
+    <t>867, 825, 873, 823, 850, 919, 931, 869, 868, 872</t>
+  </si>
+  <si>
+    <t>surrey</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50233738</t>
+  </si>
+  <si>
+    <t>25/09/23</t>
+  </si>
+  <si>
+    <t>29/09/23</t>
+  </si>
+  <si>
+    <t>25/09/26</t>
+  </si>
+  <si>
+    <t>80570</t>
+  </si>
+  <si>
+    <t>894</t>
+  </si>
+  <si>
+    <t>E06000020</t>
+  </si>
+  <si>
+    <t>371, 332, 888, 887, 813, 874, 879, 372, 866, 359</t>
+  </si>
+  <si>
+    <t>telford &amp; wrekin</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50221953</t>
+  </si>
+  <si>
+    <t>26/05/2017</t>
+  </si>
+  <si>
+    <t>20/03/28</t>
+  </si>
+  <si>
+    <t>80573</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>E08000009</t>
+  </si>
+  <si>
+    <t>867, 305, 825, 823, 895, 850, 919, 334, 356, 816</t>
+  </si>
+  <si>
+    <t>trafford</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50236174</t>
+  </si>
+  <si>
+    <t>16/10/23</t>
+  </si>
+  <si>
+    <t>20/10/23</t>
+  </si>
+  <si>
+    <t>22/12/23</t>
+  </si>
+  <si>
+    <t>16/10/26</t>
+  </si>
+  <si>
+    <t>80575</t>
+  </si>
+  <si>
+    <t>877</t>
+  </si>
+  <si>
+    <t>E06000007</t>
+  </si>
+  <si>
+    <t>351, 895, 896, 811, 881, 891, 334, 860, 356, 937</t>
+  </si>
+  <si>
+    <t>warrington</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50215729</t>
+  </si>
+  <si>
+    <t>14/12/2018</t>
+  </si>
+  <si>
+    <t>2637548</t>
+  </si>
+  <si>
+    <t>941</t>
+  </si>
+  <si>
+    <t>E06000062</t>
+  </si>
+  <si>
+    <t>822, 881, 886, 887, 940, 891, 860, 866, 937, 885</t>
+  </si>
+  <si>
+    <t>west northamptonshire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50252240</t>
+  </si>
+  <si>
+    <t>18/09/25</t>
+  </si>
+  <si>
+    <t>80578</t>
+  </si>
+  <si>
+    <t>938</t>
+  </si>
+  <si>
+    <t>E10000032</t>
+  </si>
+  <si>
+    <t>800, 823, 881, 916, 850, 855, 802, 803, 865, 885</t>
+  </si>
+  <si>
+    <t>west sussex</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50240577</t>
+  </si>
+  <si>
+    <t>27/11/23</t>
+  </si>
+  <si>
+    <t>01/12/23</t>
+  </si>
+  <si>
+    <t>29/02/24</t>
+  </si>
+  <si>
+    <t>27/11/26</t>
+  </si>
+  <si>
+    <t>80580</t>
+  </si>
+  <si>
+    <t>865</t>
+  </si>
+  <si>
+    <t>E06000054</t>
+  </si>
+  <si>
+    <t>800, 873, 878, 838, 916, 850, 802, 893, 938, 885</t>
+  </si>
+  <si>
+    <t>wiltshire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50263759</t>
+  </si>
+  <si>
+    <t>14/10/24</t>
+  </si>
+  <si>
+    <t>18/10/24</t>
+  </si>
+  <si>
+    <t>The local area partnership’s arrangements typically lead to positive experiences and outcomes for children and young people with special educational needs and/or disabilities (SEND). The local area partnership is taking action where improvements are needed.  The next full area SEND inspection will be within five years.</t>
+  </si>
+  <si>
+    <t>80584</t>
+  </si>
+  <si>
+    <t>885</t>
+  </si>
+  <si>
+    <t>E10000034</t>
+  </si>
+  <si>
+    <t>838, 845, 881, 886, 855, 802, 803, 860, 937, 938</t>
+  </si>
+  <si>
+    <t>worcestershire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50252437</t>
+  </si>
+  <si>
+    <t>03/11/2021</t>
+  </si>
+  <si>
+    <t>22/04/24</t>
+  </si>
+  <si>
+    <t>26/04/24</t>
+  </si>
+  <si>
+    <t>15/07/24</t>
+  </si>
+  <si>
+    <t>22/10/25</t>
   </si>
   <si>
     <t>urn</t>
@@ -1591,7 +2128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1599,52 +2136,52 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>389</v>
+        <v>568</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>390</v>
+        <v>569</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>391</v>
+        <v>570</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>392</v>
+        <v>571</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>393</v>
+        <v>572</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>394</v>
+        <v>573</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>395</v>
+        <v>574</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>396</v>
+        <v>575</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>397</v>
+        <v>576</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>398</v>
+        <v>577</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>399</v>
+        <v>578</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>400</v>
+        <v>579</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>401</v>
+        <v>580</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>402</v>
+        <v>581</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>403</v>
+        <v>582</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>404</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -3463,6 +4000,975 @@
       </c>
       <c r="P37" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>389</v>
+      </c>
+      <c r="B38" t="s">
+        <v>390</v>
+      </c>
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
+        <v>391</v>
+      </c>
+      <c r="E38" t="s">
+        <v>392</v>
+      </c>
+      <c r="F38" t="s">
+        <v>393</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H38" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" t="s">
+        <v>395</v>
+      </c>
+      <c r="J38" t="s">
+        <v>396</v>
+      </c>
+      <c r="K38" t="s">
+        <v>397</v>
+      </c>
+      <c r="L38" t="s">
+        <v>191</v>
+      </c>
+      <c r="M38" t="s">
+        <v>63</v>
+      </c>
+      <c r="N38" t="s">
+        <v>398</v>
+      </c>
+      <c r="O38" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80534_nottinghamshire", ".\export_data\inspection_reports\80534_nottinghamshire")</f>
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>400</v>
+      </c>
+      <c r="B39" t="s">
+        <v>401</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>402</v>
+      </c>
+      <c r="E39" t="s">
+        <v>403</v>
+      </c>
+      <c r="F39" t="s">
+        <v>404</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" t="s">
+        <v>315</v>
+      </c>
+      <c r="J39" t="s">
+        <v>406</v>
+      </c>
+      <c r="K39" t="s">
+        <v>407</v>
+      </c>
+      <c r="L39" t="s">
+        <v>408</v>
+      </c>
+      <c r="M39" t="s">
+        <v>63</v>
+      </c>
+      <c r="N39" t="s">
+        <v>409</v>
+      </c>
+      <c r="O39" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80535_oldham", ".\export_data\inspection_reports\80535_oldham")</f>
+        <v>0</v>
+      </c>
+      <c r="P39" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>410</v>
+      </c>
+      <c r="B40" t="s">
+        <v>411</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>412</v>
+      </c>
+      <c r="E40" t="s">
+        <v>413</v>
+      </c>
+      <c r="F40" t="s">
+        <v>414</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40" t="s">
+        <v>223</v>
+      </c>
+      <c r="J40" t="s">
+        <v>416</v>
+      </c>
+      <c r="K40" t="s">
+        <v>417</v>
+      </c>
+      <c r="L40" t="s">
+        <v>418</v>
+      </c>
+      <c r="M40" t="s">
+        <v>63</v>
+      </c>
+      <c r="N40" t="s">
+        <v>419</v>
+      </c>
+      <c r="O40" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80536_oxfordshire", ".\export_data\inspection_reports\80536_oxfordshire")</f>
+        <v>0</v>
+      </c>
+      <c r="P40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>420</v>
+      </c>
+      <c r="B41" t="s">
+        <v>421</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>422</v>
+      </c>
+      <c r="E41" t="s">
+        <v>423</v>
+      </c>
+      <c r="F41" t="s">
+        <v>424</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" t="s">
+        <v>426</v>
+      </c>
+      <c r="J41" t="s">
+        <v>406</v>
+      </c>
+      <c r="K41" t="s">
+        <v>407</v>
+      </c>
+      <c r="L41" t="s">
+        <v>427</v>
+      </c>
+      <c r="M41" t="s">
+        <v>63</v>
+      </c>
+      <c r="N41" t="s">
+        <v>409</v>
+      </c>
+      <c r="O41" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80538_plymouth", ".\export_data\inspection_reports\80538_plymouth")</f>
+        <v>0</v>
+      </c>
+      <c r="P41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>428</v>
+      </c>
+      <c r="B42" t="s">
+        <v>429</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>430</v>
+      </c>
+      <c r="E42" t="s">
+        <v>431</v>
+      </c>
+      <c r="F42" t="s">
+        <v>432</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" t="s">
+        <v>434</v>
+      </c>
+      <c r="K42" t="s">
+        <v>435</v>
+      </c>
+      <c r="L42" t="s">
+        <v>108</v>
+      </c>
+      <c r="M42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N42" t="s">
+        <v>436</v>
+      </c>
+      <c r="O42" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80543_rotherham", ".\export_data\inspection_reports\80543_rotherham")</f>
+        <v>0</v>
+      </c>
+      <c r="P42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>437</v>
+      </c>
+      <c r="B43" t="s">
+        <v>438</v>
+      </c>
+      <c r="C43" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" t="s">
+        <v>439</v>
+      </c>
+      <c r="E43" t="s">
+        <v>440</v>
+      </c>
+      <c r="F43" t="s">
+        <v>441</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="H43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>275</v>
+      </c>
+      <c r="J43" t="s">
+        <v>443</v>
+      </c>
+      <c r="K43" t="s">
+        <v>277</v>
+      </c>
+      <c r="L43" t="s">
+        <v>444</v>
+      </c>
+      <c r="M43" t="s">
+        <v>12</v>
+      </c>
+      <c r="N43" t="s">
+        <v>445</v>
+      </c>
+      <c r="O43" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80547_rutland", ".\export_data\inspection_reports\80547_rutland")</f>
+        <v>0</v>
+      </c>
+      <c r="P43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>446</v>
+      </c>
+      <c r="B44" t="s">
+        <v>447</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>448</v>
+      </c>
+      <c r="E44" t="s">
+        <v>449</v>
+      </c>
+      <c r="F44" t="s">
+        <v>450</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" t="s">
+        <v>452</v>
+      </c>
+      <c r="J44" t="s">
+        <v>453</v>
+      </c>
+      <c r="K44" t="s">
+        <v>454</v>
+      </c>
+      <c r="L44" t="s">
+        <v>455</v>
+      </c>
+      <c r="M44" t="s">
+        <v>26</v>
+      </c>
+      <c r="N44" t="s">
+        <v>456</v>
+      </c>
+      <c r="O44" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80549_sandwell", ".\export_data\inspection_reports\80549_sandwell")</f>
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>457</v>
+      </c>
+      <c r="B45" t="s">
+        <v>458</v>
+      </c>
+      <c r="C45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" t="s">
+        <v>459</v>
+      </c>
+      <c r="E45" t="s">
+        <v>460</v>
+      </c>
+      <c r="F45" t="s">
+        <v>461</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="H45" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" t="s">
+        <v>463</v>
+      </c>
+      <c r="K45" t="s">
+        <v>464</v>
+      </c>
+      <c r="L45" t="s">
+        <v>465</v>
+      </c>
+      <c r="M45" t="s">
+        <v>26</v>
+      </c>
+      <c r="N45" t="s">
+        <v>466</v>
+      </c>
+      <c r="O45" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80558_southampton", ".\export_data\inspection_reports\80558_southampton")</f>
+        <v>0</v>
+      </c>
+      <c r="P45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>467</v>
+      </c>
+      <c r="B46" t="s">
+        <v>468</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>469</v>
+      </c>
+      <c r="E46" t="s">
+        <v>470</v>
+      </c>
+      <c r="F46" t="s">
+        <v>471</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" t="s">
+        <v>473</v>
+      </c>
+      <c r="J46" t="s">
+        <v>474</v>
+      </c>
+      <c r="K46" t="s">
+        <v>475</v>
+      </c>
+      <c r="L46" t="s">
+        <v>476</v>
+      </c>
+      <c r="M46" t="s">
+        <v>26</v>
+      </c>
+      <c r="N46" t="s">
+        <v>477</v>
+      </c>
+      <c r="O46" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80559_southend-on-sea", ".\export_data\inspection_reports\80559_southend-on-sea")</f>
+        <v>0</v>
+      </c>
+      <c r="P46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>478</v>
+      </c>
+      <c r="B47" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>480</v>
+      </c>
+      <c r="E47" t="s">
+        <v>481</v>
+      </c>
+      <c r="F47" t="s">
+        <v>482</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" t="s">
+        <v>484</v>
+      </c>
+      <c r="J47" t="s">
+        <v>287</v>
+      </c>
+      <c r="K47" t="s">
+        <v>224</v>
+      </c>
+      <c r="L47" t="s">
+        <v>288</v>
+      </c>
+      <c r="M47" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" t="s">
+        <v>485</v>
+      </c>
+      <c r="O47" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80564_stoke-on-trent", ".\export_data\inspection_reports\80564_stoke-on-trent")</f>
+        <v>0</v>
+      </c>
+      <c r="P47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>486</v>
+      </c>
+      <c r="B48" t="s">
+        <v>487</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>488</v>
+      </c>
+      <c r="E48" t="s">
+        <v>489</v>
+      </c>
+      <c r="F48" t="s">
+        <v>490</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H48" t="s">
+        <v>58</v>
+      </c>
+      <c r="I48" t="s">
+        <v>492</v>
+      </c>
+      <c r="J48" t="s">
+        <v>493</v>
+      </c>
+      <c r="K48" t="s">
+        <v>494</v>
+      </c>
+      <c r="L48" t="s">
+        <v>495</v>
+      </c>
+      <c r="M48" t="s">
+        <v>63</v>
+      </c>
+      <c r="N48" t="s">
+        <v>496</v>
+      </c>
+      <c r="O48" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80565_suffolk", ".\export_data\inspection_reports\80565_suffolk")</f>
+        <v>0</v>
+      </c>
+      <c r="P48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" t="s">
+        <v>497</v>
+      </c>
+      <c r="B49" t="s">
+        <v>498</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" t="s">
+        <v>499</v>
+      </c>
+      <c r="E49" t="s">
+        <v>500</v>
+      </c>
+      <c r="F49" t="s">
+        <v>501</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="H49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" t="s">
+        <v>452</v>
+      </c>
+      <c r="J49" t="s">
+        <v>503</v>
+      </c>
+      <c r="K49" t="s">
+        <v>504</v>
+      </c>
+      <c r="L49" t="s">
+        <v>179</v>
+      </c>
+      <c r="M49" t="s">
+        <v>26</v>
+      </c>
+      <c r="N49" t="s">
+        <v>505</v>
+      </c>
+      <c r="O49" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80567_surrey", ".\export_data\inspection_reports\80567_surrey")</f>
+        <v>0</v>
+      </c>
+      <c r="P49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>506</v>
+      </c>
+      <c r="B50" t="s">
+        <v>507</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" t="s">
+        <v>508</v>
+      </c>
+      <c r="E50" t="s">
+        <v>509</v>
+      </c>
+      <c r="F50" t="s">
+        <v>510</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" t="s">
+        <v>512</v>
+      </c>
+      <c r="J50" t="s">
+        <v>263</v>
+      </c>
+      <c r="K50" t="s">
+        <v>264</v>
+      </c>
+      <c r="L50" t="s">
+        <v>453</v>
+      </c>
+      <c r="M50" t="s">
+        <v>12</v>
+      </c>
+      <c r="N50" t="s">
+        <v>513</v>
+      </c>
+      <c r="O50" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80570_telford &amp; wrekin", ".\export_data\inspection_reports\80570_telford &amp; wrekin")</f>
+        <v>0</v>
+      </c>
+      <c r="P50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>514</v>
+      </c>
+      <c r="B51" t="s">
+        <v>515</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>516</v>
+      </c>
+      <c r="E51" t="s">
+        <v>517</v>
+      </c>
+      <c r="F51" t="s">
+        <v>518</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" t="s">
+        <v>520</v>
+      </c>
+      <c r="K51" t="s">
+        <v>521</v>
+      </c>
+      <c r="L51" t="s">
+        <v>522</v>
+      </c>
+      <c r="M51" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" t="s">
+        <v>523</v>
+      </c>
+      <c r="O51" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80573_trafford", ".\export_data\inspection_reports\80573_trafford")</f>
+        <v>0</v>
+      </c>
+      <c r="P51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>524</v>
+      </c>
+      <c r="B52" t="s">
+        <v>525</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>526</v>
+      </c>
+      <c r="E52" t="s">
+        <v>527</v>
+      </c>
+      <c r="F52" t="s">
+        <v>528</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" t="s">
+        <v>530</v>
+      </c>
+      <c r="J52" t="s">
+        <v>85</v>
+      </c>
+      <c r="K52" t="s">
+        <v>86</v>
+      </c>
+      <c r="L52" t="s">
+        <v>87</v>
+      </c>
+      <c r="M52" t="s">
+        <v>26</v>
+      </c>
+      <c r="N52" t="s">
+        <v>88</v>
+      </c>
+      <c r="O52" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80575_warrington", ".\export_data\inspection_reports\80575_warrington")</f>
+        <v>0</v>
+      </c>
+      <c r="P52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>531</v>
+      </c>
+      <c r="B53" t="s">
+        <v>532</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" t="s">
+        <v>533</v>
+      </c>
+      <c r="E53" t="s">
+        <v>534</v>
+      </c>
+      <c r="F53" t="s">
+        <v>535</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="H53" t="s">
+        <v>58</v>
+      </c>
+      <c r="I53" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" t="s">
+        <v>73</v>
+      </c>
+      <c r="K53" t="s">
+        <v>74</v>
+      </c>
+      <c r="L53" t="s">
+        <v>244</v>
+      </c>
+      <c r="M53" t="s">
+        <v>63</v>
+      </c>
+      <c r="N53" t="s">
+        <v>537</v>
+      </c>
+      <c r="O53" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\2637548_west northamptonshire", ".\export_data\inspection_reports\2637548_west northamptonshire")</f>
+        <v>0</v>
+      </c>
+      <c r="P53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>538</v>
+      </c>
+      <c r="B54" t="s">
+        <v>539</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" t="s">
+        <v>540</v>
+      </c>
+      <c r="E54" t="s">
+        <v>541</v>
+      </c>
+      <c r="F54" t="s">
+        <v>542</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" t="s">
+        <v>544</v>
+      </c>
+      <c r="K54" t="s">
+        <v>545</v>
+      </c>
+      <c r="L54" t="s">
+        <v>546</v>
+      </c>
+      <c r="M54" t="s">
+        <v>26</v>
+      </c>
+      <c r="N54" t="s">
+        <v>547</v>
+      </c>
+      <c r="O54" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80578_west sussex", ".\export_data\inspection_reports\80578_west sussex")</f>
+        <v>0</v>
+      </c>
+      <c r="P54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>548</v>
+      </c>
+      <c r="B55" t="s">
+        <v>549</v>
+      </c>
+      <c r="C55" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" t="s">
+        <v>550</v>
+      </c>
+      <c r="E55" t="s">
+        <v>551</v>
+      </c>
+      <c r="F55" t="s">
+        <v>552</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H55" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" t="s">
+        <v>554</v>
+      </c>
+      <c r="K55" t="s">
+        <v>555</v>
+      </c>
+      <c r="L55" t="s">
+        <v>202</v>
+      </c>
+      <c r="M55" t="s">
+        <v>266</v>
+      </c>
+      <c r="N55" t="s">
+        <v>267</v>
+      </c>
+      <c r="O55" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80580_wiltshire", ".\export_data\inspection_reports\80580_wiltshire")</f>
+        <v>0</v>
+      </c>
+      <c r="P55" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>557</v>
+      </c>
+      <c r="B56" t="s">
+        <v>558</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" t="s">
+        <v>559</v>
+      </c>
+      <c r="E56" t="s">
+        <v>560</v>
+      </c>
+      <c r="F56" t="s">
+        <v>561</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="H56" t="s">
+        <v>58</v>
+      </c>
+      <c r="I56" t="s">
+        <v>563</v>
+      </c>
+      <c r="J56" t="s">
+        <v>564</v>
+      </c>
+      <c r="K56" t="s">
+        <v>565</v>
+      </c>
+      <c r="L56" t="s">
+        <v>566</v>
+      </c>
+      <c r="M56" t="s">
+        <v>63</v>
+      </c>
+      <c r="N56" t="s">
+        <v>567</v>
+      </c>
+      <c r="O56" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80584_worcestershire", ".\export_data\inspection_reports\80584_worcestershire")</f>
+        <v>0</v>
+      </c>
+      <c r="P56" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3503,6 +5009,25 @@
     <hyperlink ref="G35" r:id="rId34"/>
     <hyperlink ref="G36" r:id="rId35"/>
     <hyperlink ref="G37" r:id="rId36"/>
+    <hyperlink ref="G38" r:id="rId37"/>
+    <hyperlink ref="G39" r:id="rId38"/>
+    <hyperlink ref="G40" r:id="rId39"/>
+    <hyperlink ref="G41" r:id="rId40"/>
+    <hyperlink ref="G42" r:id="rId41"/>
+    <hyperlink ref="G43" r:id="rId42"/>
+    <hyperlink ref="G44" r:id="rId43"/>
+    <hyperlink ref="G45" r:id="rId44"/>
+    <hyperlink ref="G46" r:id="rId45"/>
+    <hyperlink ref="G47" r:id="rId46"/>
+    <hyperlink ref="G48" r:id="rId47"/>
+    <hyperlink ref="G49" r:id="rId48"/>
+    <hyperlink ref="G50" r:id="rId49"/>
+    <hyperlink ref="G51" r:id="rId50"/>
+    <hyperlink ref="G52" r:id="rId51"/>
+    <hyperlink ref="G53" r:id="rId52"/>
+    <hyperlink ref="G54" r:id="rId53"/>
+    <hyperlink ref="G55" r:id="rId54"/>
+    <hyperlink ref="G56" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>